<commit_message>
Evaluation Part 1 👻
</commit_message>
<xml_diff>
--- a/Evaluation/Evaluation.xlsx
+++ b/Evaluation/Evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Development/python_test/Evaluation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doerrschuck/PycharmProjects/python_test/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5E29EA8-D3B5-5B45-B4EF-160949E8717C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2D182E-837B-A74E-ADE1-FEFCAB932C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="800" windowWidth="43580" windowHeight="19160" xr2:uid="{789CD50E-5BAC-444E-A3D7-1CFCEDFD3EFC}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="33600" windowHeight="18840" xr2:uid="{789CD50E-5BAC-444E-A3D7-1CFCEDFD3EFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -209,10 +209,6 @@
 FP</t>
   </si>
   <si>
-    <t>EndEvent
-FP</t>
-  </si>
-  <si>
     <t>Intermediate
 Event
 FP</t>
@@ -247,6 +243,11 @@
   <si>
     <t>EG:
 Activities
+FP</t>
+  </si>
+  <si>
+    <t>End
+Event
 FP</t>
   </si>
 </sst>
@@ -691,9 +692,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7928DE-9F2D-344D-978A-A975D7019E29}">
   <dimension ref="A1:AN51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X10" sqref="X10"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -721,7 +722,7 @@
     <col min="21" max="21" width="8.6640625" style="6" customWidth="1"/>
     <col min="22" max="22" width="4.6640625" style="2" customWidth="1"/>
     <col min="23" max="23" width="4.83203125" style="6" customWidth="1"/>
-    <col min="24" max="24" width="10.33203125" style="6" customWidth="1"/>
+    <col min="24" max="24" width="7.6640625" style="6" customWidth="1"/>
     <col min="25" max="25" width="4.6640625" style="2" customWidth="1"/>
     <col min="26" max="26" width="4.83203125" style="6" customWidth="1"/>
     <col min="27" max="27" width="14.6640625" style="6" customWidth="1"/>
@@ -785,7 +786,7 @@
         <v>51</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P1" s="9" t="s">
         <v>52</v>
@@ -794,7 +795,7 @@
         <v>51</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S1" s="9" t="s">
         <v>52</v>
@@ -803,7 +804,7 @@
         <v>51</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V1" s="9" t="s">
         <v>52</v>
@@ -812,7 +813,7 @@
         <v>51</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="Y1" s="9" t="s">
         <v>52</v>
@@ -821,7 +822,7 @@
         <v>51</v>
       </c>
       <c r="AA1" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB1" s="9" t="s">
         <v>52</v>
@@ -830,7 +831,7 @@
         <v>51</v>
       </c>
       <c r="AD1" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AE1" s="10" t="s">
         <v>52</v>
@@ -839,7 +840,7 @@
         <v>51</v>
       </c>
       <c r="AG1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AH1" s="9" t="s">
         <v>52</v>
@@ -848,7 +849,7 @@
         <v>51</v>
       </c>
       <c r="AJ1" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AK1" s="9" t="s">
         <v>52</v>
@@ -857,7 +858,7 @@
         <v>51</v>
       </c>
       <c r="AM1" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AN1" s="9" t="s">
         <v>52</v>
@@ -866,6 +867,123 @@
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
+      </c>
+      <c r="B3" s="6">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>20</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5</v>
+      </c>
+      <c r="K3" s="6">
+        <v>5</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0</v>
+      </c>
+      <c r="O3" s="6">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>3</v>
+      </c>
+      <c r="R3" s="6">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0</v>
+      </c>
+      <c r="T3" s="6">
+        <v>1</v>
+      </c>
+      <c r="U3" s="6">
+        <v>0</v>
+      </c>
+      <c r="V3" s="2">
+        <v>0</v>
+      </c>
+      <c r="W3" s="6">
+        <v>1</v>
+      </c>
+      <c r="X3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="6">
+        <v>4</v>
+      </c>
+      <c r="AG3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="6">
+        <v>3</v>
+      </c>
+      <c r="AJ3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="6">
+        <v>5</v>
+      </c>
+      <c r="AM3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
@@ -917,98 +1035,683 @@
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="B13" s="6">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6">
+        <v>9</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
+        <v>9</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>3</v>
+      </c>
+      <c r="K13" s="6">
+        <v>4</v>
+      </c>
+      <c r="L13" s="6">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="6">
+        <v>0</v>
+      </c>
+      <c r="O13" s="6">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>0</v>
+      </c>
+      <c r="R13" s="6">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <v>1</v>
+      </c>
+      <c r="T13" s="6">
+        <v>1</v>
+      </c>
+      <c r="U13" s="6">
+        <v>0</v>
+      </c>
+      <c r="V13" s="2">
+        <v>0</v>
+      </c>
+      <c r="W13" s="6">
+        <v>1</v>
+      </c>
+      <c r="X13" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="6">
+        <v>3</v>
+      </c>
+      <c r="AD13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="B14" s="6">
+        <v>6</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>7</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14" s="6">
+        <v>2</v>
+      </c>
+      <c r="L14" s="6">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>2</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0</v>
+      </c>
+      <c r="O14" s="6">
+        <v>1</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>1</v>
+      </c>
+      <c r="R14" s="6">
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0</v>
+      </c>
+      <c r="T14" s="6">
+        <v>1</v>
+      </c>
+      <c r="U14" s="6">
+        <v>0</v>
+      </c>
+      <c r="V14" s="2">
+        <v>0</v>
+      </c>
+      <c r="W14" s="6">
+        <v>1</v>
+      </c>
+      <c r="X14" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG14" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="6">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="6">
+        <v>2</v>
+      </c>
+      <c r="AM14" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="B15" s="6">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>6</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6">
+        <v>6</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2</v>
+      </c>
+      <c r="K15" s="6">
+        <v>4</v>
+      </c>
+      <c r="L15" s="6">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="6">
+        <v>1</v>
+      </c>
+      <c r="O15" s="6">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>1</v>
+      </c>
+      <c r="R15" s="6">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0</v>
+      </c>
+      <c r="T15" s="6">
+        <v>1</v>
+      </c>
+      <c r="U15" s="6">
+        <v>0</v>
+      </c>
+      <c r="V15" s="2">
+        <v>0</v>
+      </c>
+      <c r="W15" s="6">
+        <v>1</v>
+      </c>
+      <c r="X15" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="6">
+        <v>2</v>
+      </c>
+      <c r="AG15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="6">
+        <v>2</v>
+      </c>
+      <c r="AJ15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL15" s="6">
+        <v>2</v>
+      </c>
+      <c r="AM15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <v>4</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <v>8</v>
+      </c>
+      <c r="I16" s="6">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1</v>
+      </c>
+      <c r="K16" s="6">
+        <v>4</v>
+      </c>
+      <c r="L16" s="6">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+      <c r="N16" s="6">
+        <v>0</v>
+      </c>
+      <c r="O16" s="6">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>0</v>
+      </c>
+      <c r="R16" s="6">
+        <v>0</v>
+      </c>
+      <c r="S16" s="2">
+        <v>1</v>
+      </c>
+      <c r="T16" s="6">
+        <v>1</v>
+      </c>
+      <c r="U16" s="6">
+        <v>0</v>
+      </c>
+      <c r="V16" s="2">
+        <v>0</v>
+      </c>
+      <c r="W16" s="6">
+        <v>2</v>
+      </c>
+      <c r="X16" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="6">
+        <v>2</v>
+      </c>
+      <c r="AD16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="6">
+        <v>2</v>
+      </c>
+      <c r="AG16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="6">
+        <v>2</v>
+      </c>
+      <c r="AJ16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="6">
+        <v>2</v>
+      </c>
+      <c r="AM16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <v>12</v>
+      </c>
+      <c r="C17" s="6">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6">
+        <v>11</v>
+      </c>
+      <c r="F17" s="6">
+        <v>3</v>
+      </c>
+      <c r="G17" s="2">
+        <v>2</v>
+      </c>
+      <c r="H17" s="6">
+        <v>16</v>
+      </c>
+      <c r="I17" s="6">
+        <v>2</v>
+      </c>
+      <c r="J17" s="2">
+        <v>5</v>
+      </c>
+      <c r="K17" s="6">
+        <v>8</v>
+      </c>
+      <c r="L17" s="6">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1</v>
+      </c>
+      <c r="N17" s="6">
+        <v>1</v>
+      </c>
+      <c r="O17" s="6">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>5</v>
+      </c>
+      <c r="R17" s="6">
+        <v>1</v>
+      </c>
+      <c r="S17" s="2">
+        <v>1</v>
+      </c>
+      <c r="T17" s="6">
+        <v>1</v>
+      </c>
+      <c r="U17" s="6">
+        <v>0</v>
+      </c>
+      <c r="V17" s="2">
+        <v>0</v>
+      </c>
+      <c r="W17" s="6">
+        <v>1</v>
+      </c>
+      <c r="X17" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="6">
+        <v>1</v>
+      </c>
+      <c r="AJ17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="6">
+        <v>2</v>
+      </c>
+      <c r="AM17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>42</v>
       </c>
@@ -1113,6 +1816,6 @@
     <sortCondition ref="A3:A39"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel Action Part 3 🎅🏼
</commit_message>
<xml_diff>
--- a/Evaluation/Evaluation.xlsx
+++ b/Evaluation/Evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doerrschuck/PycharmProjects/python_test/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D293114-52F3-B448-9974-E60C17998C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1EC9D3-46C2-B841-9810-3ED355DB0F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{789CD50E-5BAC-444E-A3D7-1CFCEDFD3EFC}"/>
   </bookViews>
@@ -789,8 +789,8 @@
   <dimension ref="A1:AP119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U21" sqref="U21"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -9398,7 +9398,7 @@
         <v>1</v>
       </c>
       <c r="L92" s="4">
-        <f t="shared" ref="L92:L100" si="399">IF(OR(ISBLANK(K32),ISBLANK(L32), ISBLANK(M32)), "", IF(K32+M32&gt;0, K32/(K32+M32), 0))</f>
+        <f t="shared" ref="L92:L99" si="399">IF(OR(ISBLANK(K32),ISBLANK(L32), ISBLANK(M32)), "", IF(K32+M32&gt;0, K32/(K32+M32), 0))</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="M92" s="2">
@@ -9410,7 +9410,7 @@
         <v>1</v>
       </c>
       <c r="O92" s="4">
-        <f t="shared" ref="O92:O100" si="400">IF(OR(ISBLANK(N32),ISBLANK(O32), ISBLANK(P32)), "", IF(N32+P32&gt;0, N32/(N32+P32), 0))</f>
+        <f t="shared" ref="O92:O99" si="400">IF(OR(ISBLANK(N32),ISBLANK(O32), ISBLANK(P32)), "", IF(N32+P32&gt;0, N32/(N32+P32), 0))</f>
         <v>1</v>
       </c>
       <c r="P92" s="2">
@@ -9422,7 +9422,7 @@
         <v>0.75</v>
       </c>
       <c r="R92" s="4">
-        <f t="shared" ref="R92:R100" si="401">IF(OR(ISBLANK(Q32),ISBLANK(R32), ISBLANK(S32)), "", IF(Q32+S32&gt;0, Q32/(Q32+S32), 0))</f>
+        <f t="shared" ref="R92:R99" si="401">IF(OR(ISBLANK(Q32),ISBLANK(R32), ISBLANK(S32)), "", IF(Q32+S32&gt;0, Q32/(Q32+S32), 0))</f>
         <v>1</v>
       </c>
       <c r="S92" s="2">
@@ -9434,7 +9434,7 @@
         <v>1</v>
       </c>
       <c r="U92" s="4">
-        <f t="shared" ref="U92:U100" si="402">IF(OR(ISBLANK(T32),ISBLANK(U32), ISBLANK(V32)), "", IF(T32+V32&gt;0, T32/(T32+V32), 0))</f>
+        <f t="shared" ref="U92:U99" si="402">IF(OR(ISBLANK(T32),ISBLANK(U32), ISBLANK(V32)), "", IF(T32+V32&gt;0, T32/(T32+V32), 0))</f>
         <v>1</v>
       </c>
       <c r="V92" s="2">
@@ -9446,7 +9446,7 @@
         <v>1</v>
       </c>
       <c r="X92" s="4">
-        <f t="shared" ref="X92:X100" si="403">IF(OR(ISBLANK(W32),ISBLANK(X32), ISBLANK(Y32)), "", IF(W32+Y32&gt;0, W32/(W32+Y32), 0))</f>
+        <f t="shared" ref="X92:X99" si="403">IF(OR(ISBLANK(W32),ISBLANK(X32), ISBLANK(Y32)), "", IF(W32+Y32&gt;0, W32/(W32+Y32), 0))</f>
         <v>1</v>
       </c>
       <c r="Y92" s="2">
@@ -9458,7 +9458,7 @@
         <v>1</v>
       </c>
       <c r="AA92" s="4">
-        <f t="shared" ref="AA92:AA100" si="404">IF(OR(ISBLANK(Z32),ISBLANK(AA32), ISBLANK(AB32)), "", IF(Z32+AB32&gt;0, Z32/(Z32+AB32), 0))</f>
+        <f t="shared" ref="AA92:AA99" si="404">IF(OR(ISBLANK(Z32),ISBLANK(AA32), ISBLANK(AB32)), "", IF(Z32+AB32&gt;0, Z32/(Z32+AB32), 0))</f>
         <v>1</v>
       </c>
       <c r="AB92" s="2">
@@ -9470,7 +9470,7 @@
         <v>0</v>
       </c>
       <c r="AD92" s="4">
-        <f t="shared" ref="AD92:AD100" si="405">IF(OR(ISBLANK(AC32),ISBLANK(AD32), ISBLANK(AE32)), "", IF(AC32+AE32&gt;0, AC32/(AC32+AE32), 0))</f>
+        <f t="shared" ref="AD92:AD99" si="405">IF(OR(ISBLANK(AC32),ISBLANK(AD32), ISBLANK(AE32)), "", IF(AC32+AE32&gt;0, AC32/(AC32+AE32), 0))</f>
         <v>0</v>
       </c>
       <c r="AE92" s="3" t="str">
@@ -9482,7 +9482,7 @@
         <v>0</v>
       </c>
       <c r="AG92" s="4">
-        <f t="shared" ref="AG92:AG100" si="406">IF(OR(ISBLANK(AF32),ISBLANK(AG32), ISBLANK(AH32)), "", IF(AF32+AH32&gt;0, AF32/(AF32+AH32), 0))</f>
+        <f t="shared" ref="AG92:AG99" si="406">IF(OR(ISBLANK(AF32),ISBLANK(AG32), ISBLANK(AH32)), "", IF(AF32+AH32&gt;0, AF32/(AF32+AH32), 0))</f>
         <v>0</v>
       </c>
       <c r="AH92" s="2" t="str">
@@ -9494,7 +9494,7 @@
         <v>0</v>
       </c>
       <c r="AJ92" s="4">
-        <f t="shared" ref="AJ92:AJ100" si="407">IF(OR(ISBLANK(AI32),ISBLANK(AJ32), ISBLANK(AK32)), "", IF(AI32+AK32&gt;0, AI32/(AI32+AK32), 0))</f>
+        <f t="shared" ref="AJ92:AJ99" si="407">IF(OR(ISBLANK(AI32),ISBLANK(AJ32), ISBLANK(AK32)), "", IF(AI32+AK32&gt;0, AI32/(AI32+AK32), 0))</f>
         <v>0</v>
       </c>
       <c r="AK92" s="2" t="str">
@@ -9506,7 +9506,7 @@
         <v>0</v>
       </c>
       <c r="AM92" s="4">
-        <f t="shared" ref="AM92:AM100" si="408">IF(OR(ISBLANK(AL32),ISBLANK(AM32), ISBLANK(AN32)), "", IF(AL32+AN32&gt;0, AL32/(AL32+AN32), 0))</f>
+        <f t="shared" ref="AM92:AM99" si="408">IF(OR(ISBLANK(AL32),ISBLANK(AM32), ISBLANK(AN32)), "", IF(AL32+AN32&gt;0, AL32/(AL32+AN32), 0))</f>
         <v>0</v>
       </c>
       <c r="AN92" s="2" t="str">
@@ -9698,7 +9698,7 @@
         <v/>
       </c>
       <c r="F94" s="4" t="str">
-        <f t="shared" ref="F94:F100" si="436">IF(OR(ISBLANK(E34),ISBLANK(F34), ISBLANK(G34)), "", IF(E34+G34&gt;0, E34/(E34+G34), 0))</f>
+        <f t="shared" ref="F94:F99" si="436">IF(OR(ISBLANK(E34),ISBLANK(F34), ISBLANK(G34)), "", IF(E34+G34&gt;0, E34/(E34+G34), 0))</f>
         <v/>
       </c>
       <c r="G94" s="2" t="str">

</xml_diff>